<commit_message>
creer batiment et unites corrige pour fonctionner avec config parsé dans modele
-planification modifiée
</commit_message>
<xml_diff>
--- a/doc/6- Planification.xlsx
+++ b/doc/6- Planification.xlsx
@@ -786,7 +786,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,6 +805,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="37">
     <border>
@@ -1242,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1410,7 +1422,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
@@ -1430,16 +1441,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1457,8 +1470,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1810,217 +1824,217 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D8" s="117"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="117"/>
-      <c r="I8" s="117"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="118"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="117"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="118"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="117" t="s">
+      <c r="D11" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="117"/>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="118"/>
+      <c r="O11" s="118"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D12" s="117"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="117"/>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="118"/>
+      <c r="N12" s="118"/>
+      <c r="O12" s="118"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
-      <c r="J13" s="117"/>
-      <c r="K13" s="117"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="118"/>
+      <c r="M13" s="118"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="117" t="s">
+      <c r="D15" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
-      <c r="G15" s="117"/>
-      <c r="H15" s="117"/>
-      <c r="I15" s="117"/>
-      <c r="J15" s="117"/>
-      <c r="K15" s="117"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
-      <c r="N15" s="117"/>
-      <c r="O15" s="117"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="117"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="117"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="117"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="117"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="117"/>
-      <c r="O17" s="117"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="118"/>
     </row>
     <row r="20" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="117" t="s">
+      <c r="D20" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="117"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="117"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="117"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="118"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="118"/>
+      <c r="K20" s="118"/>
+      <c r="L20" s="118"/>
+      <c r="M20" s="118"/>
+      <c r="N20" s="118"/>
+      <c r="O20" s="118"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="117"/>
-      <c r="I21" s="117"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="117"/>
-      <c r="L21" s="117"/>
-      <c r="M21" s="117"/>
-      <c r="N21" s="117"/>
-      <c r="O21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="118"/>
+      <c r="O21" s="118"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D22" s="117"/>
-      <c r="E22" s="117"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="117"/>
-      <c r="L22" s="117"/>
-      <c r="M22" s="117"/>
-      <c r="N22" s="117"/>
-      <c r="O22" s="117"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="118"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D23" s="117"/>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117"/>
-      <c r="G23" s="117"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="117"/>
-      <c r="J23" s="117"/>
-      <c r="K23" s="117"/>
-      <c r="L23" s="117"/>
-      <c r="M23" s="117"/>
-      <c r="N23" s="117"/>
-      <c r="O23" s="117"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="118"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="118"/>
+      <c r="M23" s="118"/>
+      <c r="N23" s="118"/>
+      <c r="O23" s="118"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D24" s="117"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="117"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="117"/>
-      <c r="L24" s="117"/>
-      <c r="M24" s="117"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="117"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="118"/>
+      <c r="M24" s="118"/>
+      <c r="N24" s="118"/>
+      <c r="O24" s="118"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -2079,7 +2093,7 @@
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="119" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="42" t="s">
@@ -2093,7 +2107,7 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="118"/>
+      <c r="C6" s="119"/>
       <c r="D6" s="45" t="s">
         <v>36</v>
       </c>
@@ -2105,7 +2119,7 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="118"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="45" t="s">
         <v>39</v>
       </c>
@@ -2117,7 +2131,7 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="118"/>
+      <c r="C8" s="119"/>
       <c r="D8" s="45" t="s">
         <v>44</v>
       </c>
@@ -2129,7 +2143,7 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="118"/>
+      <c r="C9" s="119"/>
       <c r="D9" s="45" t="s">
         <v>52</v>
       </c>
@@ -2141,7 +2155,7 @@
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="118"/>
+      <c r="C10" s="119"/>
       <c r="D10" s="45" t="s">
         <v>54</v>
       </c>
@@ -2153,7 +2167,7 @@
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="118"/>
+      <c r="C11" s="119"/>
       <c r="D11" s="45" t="s">
         <v>56</v>
       </c>
@@ -2165,7 +2179,7 @@
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="118"/>
+      <c r="C12" s="119"/>
       <c r="D12" s="45" t="s">
         <v>58</v>
       </c>
@@ -2175,7 +2189,7 @@
       <c r="F12" s="47"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="118"/>
+      <c r="C13" s="119"/>
       <c r="D13" s="45" t="s">
         <v>59</v>
       </c>
@@ -2185,7 +2199,7 @@
       <c r="F13" s="47"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="118"/>
+      <c r="C14" s="119"/>
       <c r="D14" s="45" t="s">
         <v>60</v>
       </c>
@@ -2195,7 +2209,7 @@
       <c r="F14" s="47"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C15" s="118"/>
+      <c r="C15" s="119"/>
       <c r="D15" s="45" t="s">
         <v>62</v>
       </c>
@@ -2205,7 +2219,7 @@
       <c r="F15" s="47"/>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="118"/>
+      <c r="C16" s="119"/>
       <c r="D16" s="45" t="s">
         <v>63</v>
       </c>
@@ -2215,7 +2229,7 @@
       <c r="F16" s="47"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="118"/>
+      <c r="C17" s="119"/>
       <c r="D17" s="45" t="s">
         <v>64</v>
       </c>
@@ -2227,7 +2241,7 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="118"/>
+      <c r="C18" s="119"/>
       <c r="D18" s="65" t="s">
         <v>70</v>
       </c>
@@ -2235,30 +2249,30 @@
       <c r="F18" s="47"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="118"/>
+      <c r="C19" s="119"/>
       <c r="D19" s="45"/>
       <c r="E19" s="64"/>
       <c r="F19" s="47"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="118"/>
+      <c r="C20" s="119"/>
       <c r="D20" s="45"/>
       <c r="E20" s="64"/>
       <c r="F20" s="47"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="118"/>
+      <c r="C21" s="119"/>
       <c r="D21" s="45"/>
       <c r="F21" s="47"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="118"/>
+      <c r="C22" s="119"/>
       <c r="D22" s="48"/>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="119" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="42" t="s">
@@ -2268,7 +2282,7 @@
       <c r="F23" s="44"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C24" s="118"/>
+      <c r="C24" s="119"/>
       <c r="D24" s="45" t="s">
         <v>79</v>
       </c>
@@ -2276,55 +2290,55 @@
       <c r="F24" s="47"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C25" s="118"/>
+      <c r="C25" s="119"/>
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
       <c r="F25" s="47"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C26" s="118"/>
+      <c r="C26" s="119"/>
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
       <c r="F26" s="47"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C27" s="118"/>
+      <c r="C27" s="119"/>
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
       <c r="F27" s="47"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C28" s="118"/>
+      <c r="C28" s="119"/>
       <c r="D28" s="45"/>
       <c r="E28" s="46"/>
       <c r="F28" s="47"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C29" s="118"/>
+      <c r="C29" s="119"/>
       <c r="D29" s="45"/>
       <c r="E29" s="46"/>
       <c r="F29" s="47"/>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C30" s="118"/>
+      <c r="C30" s="119"/>
       <c r="D30" s="45"/>
       <c r="E30" s="46"/>
       <c r="F30" s="47"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C31" s="118"/>
+      <c r="C31" s="119"/>
       <c r="D31" s="45"/>
       <c r="E31" s="46"/>
       <c r="F31" s="47"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="118"/>
+      <c r="C32" s="119"/>
       <c r="D32" s="48"/>
       <c r="E32" s="49"/>
       <c r="F32" s="50"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C33" s="118" t="s">
+      <c r="C33" s="119" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -2338,7 +2352,7 @@
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C34" s="118"/>
+      <c r="C34" s="119"/>
       <c r="D34" s="45" t="s">
         <v>69</v>
       </c>
@@ -2350,7 +2364,7 @@
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C35" s="118"/>
+      <c r="C35" s="119"/>
       <c r="D35" s="45" t="s">
         <v>71</v>
       </c>
@@ -2360,7 +2374,7 @@
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C36" s="118"/>
+      <c r="C36" s="119"/>
       <c r="D36" s="45" t="s">
         <v>78</v>
       </c>
@@ -2368,7 +2382,7 @@
       <c r="F36" s="47"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C37" s="118"/>
+      <c r="C37" s="119"/>
       <c r="D37" s="85" t="s">
         <v>81</v>
       </c>
@@ -2376,13 +2390,13 @@
       <c r="F37" s="47"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C38" s="118"/>
+      <c r="C38" s="119"/>
       <c r="D38" s="45"/>
       <c r="E38" s="46"/>
       <c r="F38" s="47"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C39" s="118"/>
+      <c r="C39" s="119"/>
       <c r="D39" s="48"/>
       <c r="E39" s="49"/>
       <c r="F39" s="50"/>
@@ -2520,11 +2534,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
     </row>
     <row r="4" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="120"/>
@@ -2973,6 +2987,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="E42:F42"/>
@@ -2980,11 +2999,6 @@
     <mergeCell ref="E54:F54"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="E65:F65"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -3270,16 +3284,16 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="52"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
     </row>
     <row r="3" spans="2:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="61"/>
@@ -3829,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3851,35 +3865,35 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
     </row>
     <row r="8" spans="2:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3903,10 +3917,10 @@
       <c r="C10" t="s">
         <v>219</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D10" s="127" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="107" t="s">
+      <c r="E10" s="106" t="s">
         <v>146</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -3915,7 +3929,7 @@
       <c r="G10" s="7">
         <v>1</v>
       </c>
-      <c r="H10" s="114">
+      <c r="H10" s="113">
         <v>1</v>
       </c>
     </row>
@@ -3923,10 +3937,10 @@
       <c r="C11" s="66" t="s">
         <v>222</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="128" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="108" t="s">
+      <c r="E11" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -3935,7 +3949,7 @@
       <c r="G11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="115">
+      <c r="H11" s="114">
         <v>1</v>
       </c>
       <c r="I11"/>
@@ -3944,10 +3958,10 @@
       <c r="C12" t="s">
         <v>219</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="128" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -3956,7 +3970,7 @@
       <c r="G12" s="5">
         <v>1</v>
       </c>
-      <c r="H12" s="115">
+      <c r="H12" s="114">
         <v>1</v>
       </c>
     </row>
@@ -3964,10 +3978,10 @@
       <c r="C13" t="s">
         <v>221</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="128" t="s">
         <v>150</v>
       </c>
-      <c r="E13" s="108" t="s">
+      <c r="E13" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -3976,7 +3990,7 @@
       <c r="G13" s="5">
         <v>1</v>
       </c>
-      <c r="H13" s="115">
+      <c r="H13" s="114">
         <v>1</v>
       </c>
     </row>
@@ -3984,10 +3998,10 @@
       <c r="C14" t="s">
         <v>222</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="108" t="s">
+      <c r="E14" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -3996,7 +4010,7 @@
       <c r="G14" s="5">
         <v>1</v>
       </c>
-      <c r="H14" s="115">
+      <c r="H14" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4004,22 +4018,22 @@
       <c r="C15" t="s">
         <v>224</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="128" t="s">
         <v>207</v>
       </c>
-      <c r="E15" s="108"/>
+      <c r="E15" s="107"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="115"/>
+      <c r="H15" s="114"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="104" t="s">
+      <c r="D16" s="128" t="s">
         <v>153</v>
       </c>
-      <c r="E16" s="108" t="s">
+      <c r="E16" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -4028,7 +4042,7 @@
       <c r="G16" s="5">
         <v>1</v>
       </c>
-      <c r="H16" s="115">
+      <c r="H16" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4036,10 +4050,10 @@
       <c r="C17" t="s">
         <v>222</v>
       </c>
-      <c r="D17" s="104" t="s">
+      <c r="D17" s="128" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="108" t="s">
+      <c r="E17" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -4048,7 +4062,7 @@
       <c r="G17" s="5">
         <v>1</v>
       </c>
-      <c r="H17" s="115">
+      <c r="H17" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4056,10 +4070,10 @@
       <c r="C18" t="s">
         <v>220</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="108" t="s">
+      <c r="E18" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -4068,7 +4082,7 @@
       <c r="G18" s="5">
         <v>1</v>
       </c>
-      <c r="H18" s="115">
+      <c r="H18" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4076,10 +4090,10 @@
       <c r="C19" t="s">
         <v>218</v>
       </c>
-      <c r="D19" s="104" t="s">
+      <c r="D19" s="128" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="108" t="s">
+      <c r="E19" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -4088,7 +4102,7 @@
       <c r="G19" s="5">
         <v>1</v>
       </c>
-      <c r="H19" s="115">
+      <c r="H19" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4096,22 +4110,22 @@
       <c r="C20" t="s">
         <v>218</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="E20" s="127"/>
+      <c r="E20" s="117"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="115"/>
+      <c r="H20" s="114"/>
     </row>
     <row r="21" spans="3:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="104" t="s">
+      <c r="D21" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="E21" s="107" t="s">
+      <c r="E21" s="106" t="s">
         <v>146</v>
       </c>
       <c r="F21" s="7" t="s">
@@ -4120,7 +4134,7 @@
       <c r="G21" s="7">
         <v>1</v>
       </c>
-      <c r="H21" s="115">
+      <c r="H21" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4128,10 +4142,10 @@
       <c r="C22" t="s">
         <v>222</v>
       </c>
-      <c r="D22" s="104" t="s">
+      <c r="D22" s="128" t="s">
         <v>159</v>
       </c>
-      <c r="E22" s="108" t="s">
+      <c r="E22" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F22" s="7" t="s">
@@ -4140,7 +4154,7 @@
       <c r="G22" s="5">
         <v>1</v>
       </c>
-      <c r="H22" s="115">
+      <c r="H22" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4148,10 +4162,10 @@
       <c r="C23" t="s">
         <v>225</v>
       </c>
-      <c r="D23" s="104" t="s">
+      <c r="D23" s="103" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="108" t="s">
+      <c r="E23" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F23" s="7" t="s">
@@ -4160,7 +4174,7 @@
       <c r="G23" s="5">
         <v>1</v>
       </c>
-      <c r="H23" s="115">
+      <c r="H23" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4168,10 +4182,10 @@
       <c r="C24" t="s">
         <v>219</v>
       </c>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="108" t="s">
+      <c r="E24" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -4180,7 +4194,7 @@
       <c r="G24" s="5">
         <v>1</v>
       </c>
-      <c r="H24" s="115">
+      <c r="H24" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4188,10 +4202,10 @@
       <c r="C25" t="s">
         <v>220</v>
       </c>
-      <c r="D25" s="116" t="s">
+      <c r="D25" s="115" t="s">
         <v>160</v>
       </c>
-      <c r="E25" s="108" t="s">
+      <c r="E25" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -4200,7 +4214,7 @@
       <c r="G25" s="5">
         <v>1</v>
       </c>
-      <c r="H25" s="115">
+      <c r="H25" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4208,10 +4222,10 @@
       <c r="C26" t="s">
         <v>221</v>
       </c>
-      <c r="D26" s="104" t="s">
+      <c r="D26" s="129" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="108" t="s">
+      <c r="E26" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -4220,7 +4234,7 @@
       <c r="G26" s="5">
         <v>1</v>
       </c>
-      <c r="H26" s="115">
+      <c r="H26" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4228,10 +4242,10 @@
       <c r="C27" t="s">
         <v>221</v>
       </c>
-      <c r="D27" s="104" t="s">
+      <c r="D27" s="103" t="s">
         <v>162</v>
       </c>
-      <c r="E27" s="108" t="s">
+      <c r="E27" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -4240,7 +4254,7 @@
       <c r="G27" s="5">
         <v>1</v>
       </c>
-      <c r="H27" s="115">
+      <c r="H27" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4248,10 +4262,10 @@
       <c r="C28" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="128" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="108" t="s">
+      <c r="E28" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F28" s="7" t="s">
@@ -4260,7 +4274,7 @@
       <c r="G28" s="5">
         <v>1</v>
       </c>
-      <c r="H28" s="115">
+      <c r="H28" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4268,10 +4282,10 @@
       <c r="C29" t="s">
         <v>225</v>
       </c>
-      <c r="D29" s="104" t="s">
+      <c r="D29" s="128" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="108" t="s">
+      <c r="E29" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F29" s="7" t="s">
@@ -4280,7 +4294,7 @@
       <c r="G29" s="5">
         <v>1</v>
       </c>
-      <c r="H29" s="115">
+      <c r="H29" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4288,10 +4302,10 @@
       <c r="C30" t="s">
         <v>220</v>
       </c>
-      <c r="D30" s="104" t="s">
+      <c r="D30" s="128" t="s">
         <v>163</v>
       </c>
-      <c r="E30" s="108" t="s">
+      <c r="E30" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -4300,7 +4314,7 @@
       <c r="G30" s="5">
         <v>1</v>
       </c>
-      <c r="H30" s="115">
+      <c r="H30" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4308,10 +4322,10 @@
       <c r="C31" t="s">
         <v>220</v>
       </c>
-      <c r="D31" s="104" t="s">
+      <c r="D31" s="128" t="s">
         <v>164</v>
       </c>
-      <c r="E31" s="107" t="s">
+      <c r="E31" s="106" t="s">
         <v>146</v>
       </c>
       <c r="F31" s="7" t="s">
@@ -4320,7 +4334,7 @@
       <c r="G31" s="7">
         <v>1</v>
       </c>
-      <c r="H31" s="115">
+      <c r="H31" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4328,10 +4342,10 @@
       <c r="C32" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="D32" s="104" t="s">
+      <c r="D32" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="108" t="s">
+      <c r="E32" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F32" s="7" t="s">
@@ -4340,7 +4354,7 @@
       <c r="G32" s="5">
         <v>1</v>
       </c>
-      <c r="H32" s="115">
+      <c r="H32" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4348,17 +4362,17 @@
       <c r="C33" t="s">
         <v>225</v>
       </c>
-      <c r="D33" s="104" t="s">
+      <c r="D33" s="103" t="s">
         <v>196</v>
       </c>
-      <c r="E33" s="108"/>
+      <c r="E33" s="107"/>
       <c r="F33" s="6" t="s">
         <v>174</v>
       </c>
       <c r="G33" s="5">
         <v>1</v>
       </c>
-      <c r="H33" s="115">
+      <c r="H33" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4366,10 +4380,10 @@
       <c r="C34" t="s">
         <v>222</v>
       </c>
-      <c r="D34" s="104" t="s">
+      <c r="D34" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="E34" s="108" t="s">
+      <c r="E34" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -4378,7 +4392,7 @@
       <c r="G34" s="5">
         <v>1</v>
       </c>
-      <c r="H34" s="115">
+      <c r="H34" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4386,34 +4400,34 @@
       <c r="C35" t="s">
         <v>222</v>
       </c>
-      <c r="D35" s="104" t="s">
+      <c r="D35" s="128" t="s">
         <v>212</v>
       </c>
-      <c r="E35" s="108" t="s">
+      <c r="E35" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5">
         <v>2</v>
       </c>
-      <c r="H35" s="115"/>
+      <c r="H35" s="114"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D36" s="104" t="s">
+      <c r="D36" s="103" t="s">
         <v>210</v>
       </c>
-      <c r="E36" s="108" t="s">
+      <c r="E36" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-      <c r="H36" s="115"/>
+      <c r="H36" s="114"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D37" s="104" t="s">
+      <c r="D37" s="103" t="s">
         <v>166</v>
       </c>
-      <c r="E37" s="108" t="s">
+      <c r="E37" s="107" t="s">
         <v>146</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -4422,15 +4436,15 @@
       <c r="G37" s="5">
         <v>1</v>
       </c>
-      <c r="H37" s="115">
+      <c r="H37" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D38" s="104" t="s">
+      <c r="D38" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="E38" s="108" t="s">
+      <c r="E38" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -4439,15 +4453,15 @@
       <c r="G38" s="5">
         <v>1</v>
       </c>
-      <c r="H38" s="115">
+      <c r="H38" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D39" s="104" t="s">
+      <c r="D39" s="103" t="s">
         <v>180</v>
       </c>
-      <c r="E39" s="108" t="s">
+      <c r="E39" s="107" t="s">
         <v>179</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -4456,15 +4470,15 @@
       <c r="G39" s="5">
         <v>1</v>
       </c>
-      <c r="H39" s="115">
+      <c r="H39" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D40" s="104" t="s">
+      <c r="D40" s="103" t="s">
         <v>181</v>
       </c>
-      <c r="E40" s="108" t="s">
+      <c r="E40" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -4473,15 +4487,15 @@
       <c r="G40" s="5">
         <v>2</v>
       </c>
-      <c r="H40" s="115">
+      <c r="H40" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D41" s="104" t="s">
+      <c r="D41" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="E41" s="108" t="s">
+      <c r="E41" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -4490,15 +4504,15 @@
       <c r="G41" s="5">
         <v>2</v>
       </c>
-      <c r="H41" s="115">
+      <c r="H41" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D42" s="104" t="s">
+      <c r="D42" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="E42" s="108" t="s">
+      <c r="E42" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -4507,15 +4521,15 @@
       <c r="G42" s="5">
         <v>2</v>
       </c>
-      <c r="H42" s="115">
+      <c r="H42" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D43" s="104" t="s">
+      <c r="D43" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="E43" s="108" t="s">
+      <c r="E43" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F43" s="5" t="s">
@@ -4524,15 +4538,15 @@
       <c r="G43" s="5">
         <v>2</v>
       </c>
-      <c r="H43" s="115">
+      <c r="H43" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D44" s="104" t="s">
+      <c r="D44" s="103" t="s">
         <v>184</v>
       </c>
-      <c r="E44" s="108" t="s">
+      <c r="E44" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F44" s="5" t="s">
@@ -4541,15 +4555,15 @@
       <c r="G44" s="5">
         <v>2</v>
       </c>
-      <c r="H44" s="115">
+      <c r="H44" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D45" s="104" t="s">
+      <c r="D45" s="103" t="s">
         <v>186</v>
       </c>
-      <c r="E45" s="108" t="s">
+      <c r="E45" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F45" s="5" t="s">
@@ -4558,15 +4572,15 @@
       <c r="G45" s="5">
         <v>2</v>
       </c>
-      <c r="H45" s="115">
+      <c r="H45" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D46" s="104" t="s">
+      <c r="D46" s="103" t="s">
         <v>187</v>
       </c>
-      <c r="E46" s="108" t="s">
+      <c r="E46" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -4575,15 +4589,15 @@
       <c r="G46" s="5">
         <v>2</v>
       </c>
-      <c r="H46" s="115">
+      <c r="H46" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D47" s="104" t="s">
+      <c r="D47" s="103" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="108" t="s">
+      <c r="E47" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F47" s="5" t="s">
@@ -4592,15 +4606,15 @@
       <c r="G47" s="5">
         <v>2</v>
       </c>
-      <c r="H47" s="115">
+      <c r="H47" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D48" s="104" t="s">
+      <c r="D48" s="103" t="s">
         <v>189</v>
       </c>
-      <c r="E48" s="108" t="s">
+      <c r="E48" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F48" s="5" t="s">
@@ -4609,15 +4623,15 @@
       <c r="G48" s="5">
         <v>2</v>
       </c>
-      <c r="H48" s="115">
+      <c r="H48" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D49" s="104" t="s">
+      <c r="D49" s="103" t="s">
         <v>190</v>
       </c>
-      <c r="E49" s="108" t="s">
+      <c r="E49" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F49" s="5" t="s">
@@ -4626,15 +4640,15 @@
       <c r="G49" s="5">
         <v>2</v>
       </c>
-      <c r="H49" s="115">
+      <c r="H49" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D50" s="104" t="s">
+      <c r="D50" s="103" t="s">
         <v>191</v>
       </c>
-      <c r="E50" s="108" t="s">
+      <c r="E50" s="107" t="s">
         <v>169</v>
       </c>
       <c r="F50" s="5" t="s">
@@ -4643,75 +4657,75 @@
       <c r="G50" s="5">
         <v>2</v>
       </c>
-      <c r="H50" s="115">
+      <c r="H50" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D51" s="105" t="s">
+      <c r="D51" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="E51" s="108" t="s">
+      <c r="E51" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="F51" s="106" t="s">
+      <c r="F51" s="105" t="s">
         <v>174</v>
       </c>
       <c r="G51" s="5">
         <v>2</v>
       </c>
-      <c r="H51" s="115">
+      <c r="H51" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D52" s="105" t="s">
+      <c r="D52" s="104" t="s">
         <v>193</v>
       </c>
-      <c r="E52" s="108" t="s">
+      <c r="E52" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="F52" s="106" t="s">
+      <c r="F52" s="105" t="s">
         <v>204</v>
       </c>
       <c r="G52" s="5">
         <v>2</v>
       </c>
-      <c r="H52" s="115">
+      <c r="H52" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D53" s="105" t="s">
+      <c r="D53" s="104" t="s">
         <v>200</v>
       </c>
-      <c r="E53" s="109" t="s">
+      <c r="E53" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="F53" s="106" t="s">
+      <c r="F53" s="105" t="s">
         <v>203</v>
       </c>
-      <c r="G53" s="106">
+      <c r="G53" s="105">
         <v>3</v>
       </c>
-      <c r="H53" s="115">
+      <c r="H53" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D54" s="106" t="s">
+      <c r="D54" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="E54" s="106" t="s">
+      <c r="E54" s="105" t="s">
         <v>179</v>
       </c>
-      <c r="F54" s="106" t="s">
+      <c r="F54" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="G54" s="106">
+      <c r="G54" s="105">
         <v>3</v>
       </c>
-      <c r="H54" s="115">
+      <c r="H54" s="114">
         <v>1</v>
       </c>
     </row>
@@ -4728,12 +4742,12 @@
       <c r="G55" s="5">
         <v>3</v>
       </c>
-      <c r="H55" s="115">
+      <c r="H55" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D56" s="126" t="s">
+      <c r="D56" s="116" t="s">
         <v>208</v>
       </c>
       <c r="E56" s="5" t="s">
@@ -4745,12 +4759,12 @@
       <c r="G56" s="5">
         <v>3</v>
       </c>
-      <c r="H56" s="115">
+      <c r="H56" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D57" s="126" t="s">
+      <c r="D57" s="116" t="s">
         <v>209</v>
       </c>
       <c r="E57" s="5" t="s">
@@ -4762,12 +4776,12 @@
       <c r="G57" s="5">
         <v>3</v>
       </c>
-      <c r="H57" s="115">
+      <c r="H57" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D58" s="126" t="s">
+      <c r="D58" s="116" t="s">
         <v>211</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -4779,12 +4793,12 @@
       <c r="G58" s="5">
         <v>3</v>
       </c>
-      <c r="H58" s="115">
+      <c r="H58" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D59" s="126" t="s">
+      <c r="D59" s="116" t="s">
         <v>213</v>
       </c>
       <c r="E59" s="5" t="s">
@@ -4796,7 +4810,7 @@
       <c r="G59" s="5">
         <v>3</v>
       </c>
-      <c r="H59" s="115">
+      <c r="H59" s="114">
         <v>1</v>
       </c>
     </row>
@@ -5021,8 +5035,8 @@
       <c r="C14" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="113"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="112"/>
       <c r="F14" s="63"/>
       <c r="G14" s="62"/>
       <c r="H14" s="36"/>
@@ -5034,8 +5048,8 @@
       <c r="C15" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="113"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="112"/>
       <c r="F15" s="63"/>
       <c r="G15" s="62"/>
       <c r="H15" s="36"/>
@@ -5047,8 +5061,8 @@
       <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="110"/>
-      <c r="E16" s="113"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="112"/>
       <c r="F16" s="63"/>
       <c r="G16" s="62"/>
       <c r="H16" s="36"/>
@@ -5061,8 +5075,8 @@
         <v>106</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="113"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="112"/>
       <c r="F17" s="63"/>
       <c r="G17" s="62"/>
       <c r="H17" s="36"/>
@@ -5074,8 +5088,8 @@
       <c r="C18" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="113"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="112"/>
       <c r="F18" s="63"/>
       <c r="G18" s="62"/>
       <c r="H18" s="36"/>
@@ -5087,8 +5101,8 @@
       <c r="C19" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="110"/>
-      <c r="E19" s="113"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="112"/>
       <c r="F19" s="63"/>
       <c r="G19" s="62"/>
       <c r="H19" s="36"/>
@@ -5101,8 +5115,8 @@
         <v>94</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="113"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="112"/>
       <c r="F20" s="63"/>
       <c r="G20" s="62"/>
       <c r="H20" s="36"/>
@@ -5114,8 +5128,8 @@
       <c r="C21" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="110"/>
-      <c r="E21" s="113"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="112"/>
       <c r="F21" s="63"/>
       <c r="G21" s="62"/>
       <c r="H21" s="36"/>
@@ -5128,8 +5142,8 @@
         <v>112</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="113"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="112"/>
       <c r="F22" s="63"/>
       <c r="G22" s="62"/>
       <c r="H22" s="36"/>
@@ -5141,8 +5155,8 @@
       <c r="C23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="110"/>
-      <c r="E23" s="113"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="112"/>
       <c r="F23" s="63"/>
       <c r="G23" s="62"/>
       <c r="H23" s="36"/>
@@ -5155,8 +5169,8 @@
         <v>92</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="113"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="112"/>
       <c r="F24" s="63"/>
       <c r="G24" s="62"/>
       <c r="H24" s="36"/>
@@ -5168,8 +5182,8 @@
       <c r="C25" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="110"/>
-      <c r="E25" s="113"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="112"/>
       <c r="F25" s="63"/>
       <c r="G25" s="62"/>
       <c r="H25" s="36"/>
@@ -5181,8 +5195,8 @@
       <c r="C26" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="110"/>
-      <c r="E26" s="113"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="112"/>
       <c r="F26" s="63"/>
       <c r="G26" s="62"/>
       <c r="H26" s="36"/>
@@ -5195,8 +5209,8 @@
         <v>103</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="113"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="112"/>
       <c r="F27" s="63"/>
       <c r="G27" s="62"/>
       <c r="H27" s="36"/>
@@ -5208,8 +5222,8 @@
       <c r="C28" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="110"/>
-      <c r="E28" s="113"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="112"/>
       <c r="F28" s="63"/>
       <c r="G28" s="62"/>
       <c r="H28" s="36"/>
@@ -5222,8 +5236,8 @@
         <v>104</v>
       </c>
       <c r="C29" s="10"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="113"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="112"/>
       <c r="F29" s="63"/>
       <c r="G29" s="62"/>
       <c r="H29" s="36"/>
@@ -5235,8 +5249,8 @@
       <c r="C30" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="110"/>
-      <c r="E30" s="113"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="112"/>
       <c r="F30" s="63"/>
       <c r="G30" s="62"/>
       <c r="H30" s="36"/>
@@ -5249,8 +5263,8 @@
         <v>116</v>
       </c>
       <c r="C31" s="10"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="113"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="112"/>
       <c r="F31" s="63"/>
       <c r="G31" s="62"/>
       <c r="H31" s="36"/>
@@ -5262,8 +5276,8 @@
       <c r="C32" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="110"/>
-      <c r="E32" s="113"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="112"/>
       <c r="F32" s="63"/>
       <c r="G32" s="62"/>
       <c r="H32" s="36"/>
@@ -5276,8 +5290,8 @@
         <v>118</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="113"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="112"/>
       <c r="F33" s="63"/>
       <c r="G33" s="62"/>
       <c r="H33" s="36"/>
@@ -5289,8 +5303,8 @@
       <c r="C34" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="110"/>
-      <c r="E34" s="113"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="112"/>
       <c r="F34" s="63"/>
       <c r="G34" s="62"/>
       <c r="H34" s="36"/>
@@ -5303,8 +5317,8 @@
         <v>116</v>
       </c>
       <c r="C35" s="10"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="113"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="112"/>
       <c r="F35" s="63"/>
       <c r="G35" s="62"/>
       <c r="H35" s="36"/>
@@ -5316,8 +5330,8 @@
       <c r="C36" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="110"/>
-      <c r="E36" s="113"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="112"/>
       <c r="F36" s="63"/>
       <c r="G36" s="62"/>
       <c r="H36" s="36"/>
@@ -5330,8 +5344,8 @@
         <v>94</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="110"/>
-      <c r="E37" s="113"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="112"/>
       <c r="F37" s="63"/>
       <c r="G37" s="62"/>
       <c r="H37" s="36"/>
@@ -5343,8 +5357,8 @@
       <c r="C38" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="110"/>
-      <c r="E38" s="113"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="112"/>
       <c r="F38" s="63"/>
       <c r="G38" s="62"/>
       <c r="H38" s="36"/>
@@ -5357,8 +5371,8 @@
         <v>127</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="113"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="112"/>
       <c r="F39" s="63"/>
       <c r="G39" s="62"/>
       <c r="H39" s="36"/>
@@ -5370,8 +5384,8 @@
       <c r="C40" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="110"/>
-      <c r="E40" s="113"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="112"/>
       <c r="F40" s="63"/>
       <c r="G40" s="62"/>
       <c r="H40" s="36"/>
@@ -5384,7 +5398,7 @@
         <v>90</v>
       </c>
       <c r="C41" s="10"/>
-      <c r="D41" s="110"/>
+      <c r="D41" s="109"/>
       <c r="E41" s="36"/>
       <c r="F41" s="63"/>
       <c r="G41" s="62"/>
@@ -5397,12 +5411,12 @@
       <c r="C42" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="110"/>
-      <c r="E42" s="113"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="112"/>
       <c r="F42" s="63"/>
       <c r="G42" s="62"/>
       <c r="H42" s="36"/>
-      <c r="I42" s="112"/>
+      <c r="I42" s="111"/>
       <c r="K42" s="36"/>
       <c r="N42" s="36"/>
     </row>
@@ -5411,12 +5425,12 @@
       <c r="C43" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="110"/>
-      <c r="E43" s="113"/>
+      <c r="D43" s="109"/>
+      <c r="E43" s="112"/>
       <c r="F43" s="63"/>
       <c r="G43" s="62"/>
       <c r="H43" s="36"/>
-      <c r="I43" s="112"/>
+      <c r="I43" s="111"/>
       <c r="K43" s="36"/>
       <c r="N43" s="36"/>
     </row>
@@ -5426,12 +5440,12 @@
         <v>94</v>
       </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="110"/>
-      <c r="E44" s="113"/>
+      <c r="D44" s="109"/>
+      <c r="E44" s="112"/>
       <c r="F44" s="63"/>
       <c r="G44" s="62"/>
       <c r="H44" s="36"/>
-      <c r="I44" s="112"/>
+      <c r="I44" s="111"/>
       <c r="K44" s="36"/>
       <c r="N44" s="36"/>
     </row>
@@ -5440,12 +5454,12 @@
       <c r="C45" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="D45" s="110"/>
-      <c r="E45" s="113"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="112"/>
       <c r="F45" s="63"/>
       <c r="G45" s="62"/>
       <c r="H45" s="36"/>
-      <c r="I45" s="112"/>
+      <c r="I45" s="111"/>
       <c r="K45" s="36"/>
       <c r="N45" s="36"/>
     </row>
@@ -5455,11 +5469,11 @@
         <v>103</v>
       </c>
       <c r="C46" s="10"/>
-      <c r="D46" s="110"/>
-      <c r="E46" s="113"/>
+      <c r="D46" s="109"/>
+      <c r="E46" s="112"/>
       <c r="F46" s="63"/>
       <c r="H46" s="36"/>
-      <c r="I46" s="112"/>
+      <c r="I46" s="111"/>
       <c r="K46" s="36"/>
       <c r="N46" s="36"/>
     </row>
@@ -5468,12 +5482,12 @@
       <c r="C47" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="110"/>
-      <c r="E47" s="113"/>
+      <c r="D47" s="109"/>
+      <c r="E47" s="112"/>
       <c r="F47" s="63"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="112"/>
-      <c r="J47" s="112"/>
+      <c r="I47" s="111"/>
+      <c r="J47" s="111"/>
       <c r="K47" s="36"/>
       <c r="N47" s="36"/>
     </row>
@@ -5483,12 +5497,12 @@
         <v>93</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="110"/>
-      <c r="E48" s="113"/>
+      <c r="D48" s="109"/>
+      <c r="E48" s="112"/>
       <c r="F48" s="63"/>
       <c r="H48" s="36"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
+      <c r="I48" s="111"/>
+      <c r="J48" s="111"/>
       <c r="K48" s="36"/>
       <c r="N48" s="36"/>
     </row>
@@ -5497,12 +5511,12 @@
       <c r="C49" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="110"/>
-      <c r="E49" s="113"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="112"/>
       <c r="F49" s="63"/>
       <c r="H49" s="36"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="112"/>
+      <c r="I49" s="111"/>
+      <c r="J49" s="111"/>
       <c r="K49" s="36"/>
       <c r="N49" s="36"/>
     </row>
@@ -5512,12 +5526,12 @@
         <v>129</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="110"/>
-      <c r="E50" s="113"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="112"/>
       <c r="F50" s="63"/>
       <c r="H50" s="36"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
       <c r="K50" s="36"/>
       <c r="N50" s="36"/>
     </row>
@@ -5526,12 +5540,12 @@
       <c r="C51" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D51" s="110"/>
-      <c r="E51" s="113"/>
+      <c r="D51" s="109"/>
+      <c r="E51" s="112"/>
       <c r="F51" s="63"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="112"/>
-      <c r="J51" s="112"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="111"/>
       <c r="K51" s="36"/>
       <c r="N51" s="36"/>
     </row>
@@ -5541,7 +5555,7 @@
         <v>91</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="110"/>
+      <c r="D52" s="109"/>
       <c r="E52" s="36"/>
       <c r="F52" s="63"/>
       <c r="H52" s="36"/>
@@ -5553,12 +5567,12 @@
       <c r="C53" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D53" s="110"/>
-      <c r="E53" s="113"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="112"/>
       <c r="F53" s="63"/>
       <c r="H53" s="36"/>
-      <c r="I53" s="112"/>
-      <c r="J53" s="112"/>
+      <c r="I53" s="111"/>
+      <c r="J53" s="111"/>
       <c r="K53" s="36"/>
       <c r="N53" s="36"/>
     </row>
@@ -5568,8 +5582,8 @@
         <v>94</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="D54" s="110"/>
-      <c r="E54" s="113"/>
+      <c r="D54" s="109"/>
+      <c r="E54" s="112"/>
       <c r="H54" s="36"/>
       <c r="K54" s="36"/>
       <c r="N54" s="36"/>
@@ -5579,11 +5593,11 @@
       <c r="C55" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D55" s="110"/>
-      <c r="E55" s="113"/>
+      <c r="D55" s="109"/>
+      <c r="E55" s="112"/>
       <c r="H55" s="36"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="112"/>
+      <c r="I55" s="111"/>
+      <c r="J55" s="111"/>
       <c r="K55" s="36"/>
       <c r="N55" s="36"/>
     </row>
@@ -5593,11 +5607,11 @@
         <v>95</v>
       </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="110"/>
+      <c r="D56" s="109"/>
       <c r="E56" s="36"/>
       <c r="H56" s="36"/>
-      <c r="I56" s="112"/>
-      <c r="J56" s="112"/>
+      <c r="I56" s="111"/>
+      <c r="J56" s="111"/>
       <c r="K56" s="36"/>
       <c r="N56" s="36"/>
     </row>
@@ -5606,11 +5620,11 @@
       <c r="C57" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D57" s="110"/>
-      <c r="E57" s="113"/>
+      <c r="D57" s="109"/>
+      <c r="E57" s="112"/>
       <c r="H57" s="36"/>
-      <c r="I57" s="112"/>
-      <c r="J57" s="112"/>
+      <c r="I57" s="111"/>
+      <c r="J57" s="111"/>
       <c r="K57" s="36"/>
       <c r="N57" s="36"/>
     </row>
@@ -5619,11 +5633,11 @@
       <c r="C58" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D58" s="110"/>
-      <c r="E58" s="113"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="112"/>
       <c r="H58" s="36"/>
-      <c r="I58" s="112"/>
-      <c r="J58" s="112"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="111"/>
       <c r="K58" s="36"/>
       <c r="N58" s="36"/>
     </row>
@@ -5633,11 +5647,11 @@
         <v>134</v>
       </c>
       <c r="C59" s="10"/>
-      <c r="D59" s="110"/>
-      <c r="E59" s="113"/>
+      <c r="D59" s="109"/>
+      <c r="E59" s="112"/>
       <c r="H59" s="36"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
+      <c r="I59" s="111"/>
+      <c r="J59" s="111"/>
       <c r="K59" s="36"/>
       <c r="N59" s="36"/>
     </row>
@@ -5646,11 +5660,11 @@
       <c r="C60" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D60" s="110"/>
-      <c r="E60" s="113"/>
+      <c r="D60" s="109"/>
+      <c r="E60" s="112"/>
       <c r="H60" s="36"/>
-      <c r="I60" s="112"/>
-      <c r="J60" s="112"/>
+      <c r="I60" s="111"/>
+      <c r="J60" s="111"/>
       <c r="K60" s="36"/>
       <c r="N60" s="36"/>
     </row>
@@ -5659,11 +5673,11 @@
       <c r="C61" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D61" s="110"/>
-      <c r="E61" s="113"/>
+      <c r="D61" s="109"/>
+      <c r="E61" s="112"/>
       <c r="H61" s="36"/>
-      <c r="I61" s="112"/>
-      <c r="J61" s="112"/>
+      <c r="I61" s="111"/>
+      <c r="J61" s="111"/>
       <c r="K61" s="36"/>
       <c r="N61" s="36"/>
     </row>
@@ -5673,11 +5687,11 @@
         <v>98</v>
       </c>
       <c r="C62" s="10"/>
-      <c r="D62" s="110"/>
-      <c r="E62" s="113"/>
+      <c r="D62" s="109"/>
+      <c r="E62" s="112"/>
       <c r="H62" s="36"/>
-      <c r="I62" s="112"/>
-      <c r="J62" s="112"/>
+      <c r="I62" s="111"/>
+      <c r="J62" s="111"/>
       <c r="K62" s="36"/>
       <c r="N62" s="36"/>
     </row>
@@ -5686,11 +5700,11 @@
       <c r="C63" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D63" s="110"/>
-      <c r="E63" s="113"/>
+      <c r="D63" s="109"/>
+      <c r="E63" s="112"/>
       <c r="H63" s="36"/>
-      <c r="I63" s="112"/>
-      <c r="J63" s="112"/>
+      <c r="I63" s="111"/>
+      <c r="J63" s="111"/>
       <c r="K63" s="36"/>
       <c r="N63" s="36"/>
     </row>
@@ -5699,11 +5713,11 @@
       <c r="C64" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D64" s="110"/>
-      <c r="E64" s="113"/>
+      <c r="D64" s="109"/>
+      <c r="E64" s="112"/>
       <c r="H64" s="36"/>
-      <c r="I64" s="112"/>
-      <c r="J64" s="112"/>
+      <c r="I64" s="111"/>
+      <c r="J64" s="111"/>
       <c r="K64" s="36"/>
       <c r="N64" s="36"/>
     </row>
@@ -5713,11 +5727,11 @@
         <v>96</v>
       </c>
       <c r="C65" s="10"/>
-      <c r="D65" s="110"/>
-      <c r="E65" s="113"/>
+      <c r="D65" s="109"/>
+      <c r="E65" s="112"/>
       <c r="H65" s="36"/>
-      <c r="I65" s="112"/>
-      <c r="J65" s="112"/>
+      <c r="I65" s="111"/>
+      <c r="J65" s="111"/>
       <c r="K65" s="36"/>
       <c r="N65" s="36"/>
     </row>
@@ -5726,11 +5740,11 @@
       <c r="C66" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D66" s="110"/>
-      <c r="E66" s="113"/>
+      <c r="D66" s="109"/>
+      <c r="E66" s="112"/>
       <c r="H66" s="36"/>
-      <c r="I66" s="112"/>
-      <c r="J66" s="112"/>
+      <c r="I66" s="111"/>
+      <c r="J66" s="111"/>
       <c r="K66" s="36"/>
       <c r="N66" s="36"/>
     </row>
@@ -5740,11 +5754,11 @@
         <v>97</v>
       </c>
       <c r="C67" s="10"/>
-      <c r="D67" s="110"/>
-      <c r="E67" s="113"/>
+      <c r="D67" s="109"/>
+      <c r="E67" s="112"/>
       <c r="H67" s="36"/>
-      <c r="I67" s="112"/>
-      <c r="J67" s="112"/>
+      <c r="I67" s="111"/>
+      <c r="J67" s="111"/>
       <c r="K67" s="36"/>
       <c r="N67" s="36"/>
     </row>
@@ -5753,11 +5767,11 @@
       <c r="C68" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D68" s="110"/>
-      <c r="E68" s="113"/>
+      <c r="D68" s="109"/>
+      <c r="E68" s="112"/>
       <c r="H68" s="36"/>
-      <c r="I68" s="112"/>
-      <c r="J68" s="112"/>
+      <c r="I68" s="111"/>
+      <c r="J68" s="111"/>
       <c r="K68" s="36"/>
       <c r="N68" s="36"/>
     </row>
@@ -5767,11 +5781,11 @@
         <v>99</v>
       </c>
       <c r="C69" s="10"/>
-      <c r="D69" s="110"/>
-      <c r="E69" s="113"/>
+      <c r="D69" s="109"/>
+      <c r="E69" s="112"/>
       <c r="H69" s="36"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="112"/>
+      <c r="I69" s="111"/>
+      <c r="J69" s="111"/>
       <c r="K69" s="36"/>
       <c r="N69" s="36"/>
     </row>
@@ -5780,11 +5794,11 @@
       <c r="C70" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D70" s="110"/>
-      <c r="E70" s="113"/>
+      <c r="D70" s="109"/>
+      <c r="E70" s="112"/>
       <c r="H70" s="36"/>
-      <c r="I70" s="112"/>
-      <c r="J70" s="112"/>
+      <c r="I70" s="111"/>
+      <c r="J70" s="111"/>
       <c r="K70" s="36"/>
       <c r="N70" s="36"/>
     </row>
@@ -5793,11 +5807,11 @@
       <c r="C71" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D71" s="110"/>
-      <c r="E71" s="113"/>
+      <c r="D71" s="109"/>
+      <c r="E71" s="112"/>
       <c r="H71" s="36"/>
-      <c r="I71" s="112"/>
-      <c r="J71" s="112"/>
+      <c r="I71" s="111"/>
+      <c r="J71" s="111"/>
       <c r="K71" s="36"/>
       <c r="N71" s="36"/>
     </row>
@@ -5807,10 +5821,10 @@
         <v>100</v>
       </c>
       <c r="C72" s="10"/>
-      <c r="D72" s="110"/>
-      <c r="E72" s="113"/>
+      <c r="D72" s="109"/>
+      <c r="E72" s="112"/>
       <c r="H72" s="36"/>
-      <c r="I72" s="112"/>
+      <c r="I72" s="111"/>
       <c r="K72" s="36"/>
       <c r="N72" s="36"/>
     </row>
@@ -5819,12 +5833,12 @@
       <c r="C73" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D73" s="110"/>
-      <c r="E73" s="113"/>
+      <c r="D73" s="109"/>
+      <c r="E73" s="112"/>
       <c r="H73" s="36"/>
       <c r="K73" s="36"/>
-      <c r="L73" s="112"/>
-      <c r="M73" s="112"/>
+      <c r="L73" s="111"/>
+      <c r="M73" s="111"/>
       <c r="N73" s="36"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -5832,12 +5846,12 @@
       <c r="C74" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D74" s="110"/>
-      <c r="E74" s="113"/>
+      <c r="D74" s="109"/>
+      <c r="E74" s="112"/>
       <c r="H74" s="36"/>
       <c r="K74" s="36"/>
-      <c r="L74" s="112"/>
-      <c r="M74" s="112"/>
+      <c r="L74" s="111"/>
+      <c r="M74" s="111"/>
       <c r="N74" s="36"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -5846,12 +5860,12 @@
         <v>101</v>
       </c>
       <c r="C75" s="10"/>
-      <c r="D75" s="110"/>
-      <c r="E75" s="113"/>
+      <c r="D75" s="109"/>
+      <c r="E75" s="112"/>
       <c r="H75" s="36"/>
       <c r="K75" s="36"/>
-      <c r="L75" s="112"/>
-      <c r="M75" s="112"/>
+      <c r="L75" s="111"/>
+      <c r="M75" s="111"/>
       <c r="N75" s="36"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -5859,12 +5873,12 @@
       <c r="C76" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D76" s="110"/>
-      <c r="E76" s="113"/>
+      <c r="D76" s="109"/>
+      <c r="E76" s="112"/>
       <c r="H76" s="36"/>
       <c r="K76" s="36"/>
-      <c r="L76" s="112"/>
-      <c r="M76" s="112"/>
+      <c r="L76" s="111"/>
+      <c r="M76" s="111"/>
       <c r="N76" s="36"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -5872,12 +5886,12 @@
       <c r="C77" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D77" s="110"/>
-      <c r="E77" s="113"/>
+      <c r="D77" s="109"/>
+      <c r="E77" s="112"/>
       <c r="H77" s="36"/>
       <c r="K77" s="36"/>
-      <c r="L77" s="112"/>
-      <c r="M77" s="112"/>
+      <c r="L77" s="111"/>
+      <c r="M77" s="111"/>
       <c r="N77" s="36"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -5886,12 +5900,12 @@
         <v>102</v>
       </c>
       <c r="C78" s="10"/>
-      <c r="D78" s="110"/>
-      <c r="E78" s="113"/>
+      <c r="D78" s="109"/>
+      <c r="E78" s="112"/>
       <c r="H78" s="36"/>
       <c r="K78" s="36"/>
-      <c r="L78" s="112"/>
-      <c r="M78" s="112"/>
+      <c r="L78" s="111"/>
+      <c r="M78" s="111"/>
       <c r="N78" s="36"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -5899,19 +5913,19 @@
       <c r="C79" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D79" s="110"/>
-      <c r="E79" s="113"/>
+      <c r="D79" s="109"/>
+      <c r="E79" s="112"/>
       <c r="H79" s="36"/>
       <c r="K79" s="36"/>
-      <c r="L79" s="112"/>
-      <c r="M79" s="112"/>
+      <c r="L79" s="111"/>
+      <c r="M79" s="111"/>
       <c r="N79" s="36"/>
     </row>
     <row r="80" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="36"/>
       <c r="B80" s="39"/>
       <c r="C80" s="40"/>
-      <c r="D80" s="111"/>
+      <c r="D80" s="110"/>
       <c r="E80" s="41"/>
       <c r="F80" s="40"/>
       <c r="G80" s="40"/>

</xml_diff>